<commit_message>
Crystal RC values updated. New pcb images added
</commit_message>
<xml_diff>
--- a/Manufacturing/NB-IoT-ideaboard-v2-BoM.xlsx
+++ b/Manufacturing/NB-IoT-ideaboard-v2-BoM.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Danindu\Documents\eagle\Ideamart\STM32F103R\ideaboard\Manufacturing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8DEA5D9-9B67-4229-9748-3727E92CBCE0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29E14B66-1BC1-49D1-97B5-4906908D3EE9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{934E52F4-75EA-49A0-9062-5DB83AEAECE2}"/>
   </bookViews>
@@ -226,9 +226,6 @@
     <t>C20, C21</t>
   </si>
   <si>
-    <t>25pF</t>
-  </si>
-  <si>
     <t>C10, C11</t>
   </si>
   <si>
@@ -265,9 +262,6 @@
     <t>C24, C26, C27, C32</t>
   </si>
   <si>
-    <t>400R</t>
-  </si>
-  <si>
     <t>R9</t>
   </si>
   <si>
@@ -451,9 +445,6 @@
     <t>SOT23-6L</t>
   </si>
   <si>
-    <t>5x5mm push button SMD</t>
-  </si>
-  <si>
     <t>IFSC1515AHER2R2M01</t>
   </si>
   <si>
@@ -478,9 +469,6 @@
     <t>C1, C2, C4, C5, C6, C7, C9, C22, C23, C25, C30, C35</t>
   </si>
   <si>
-    <t>USER, NRST, PWRKEY, RESET</t>
-  </si>
-  <si>
     <t>eSIM chip MFF2</t>
   </si>
   <si>
@@ -635,6 +623,18 @@
   </si>
   <si>
     <t>CAN/USART/SPI1 and 2</t>
+  </si>
+  <si>
+    <t>330k</t>
+  </si>
+  <si>
+    <t>20pF</t>
+  </si>
+  <si>
+    <t>S2, S3, S4, S6</t>
+  </si>
+  <si>
+    <t>5x5mm push button SMD (USER, NRST, PWRKEY, RESET)</t>
   </si>
 </sst>
 </file>
@@ -1043,8 +1043,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FD574948-0478-4CFE-AC71-3AD259BA437F}">
   <dimension ref="A1:G55"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1075,10 +1075,10 @@
         <v>4</v>
       </c>
       <c r="F1" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="G1" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
@@ -1087,10 +1087,10 @@
       </c>
       <c r="B2" s="1"/>
       <c r="C2" s="1" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>7</v>
@@ -1104,10 +1104,10 @@
       </c>
       <c r="B3" s="1"/>
       <c r="C3" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>191</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>195</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>7</v>
@@ -1121,10 +1121,10 @@
       </c>
       <c r="B4" s="1"/>
       <c r="C4" s="1" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>7</v>
@@ -1189,10 +1189,10 @@
         <v>10</v>
       </c>
       <c r="D7" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="E7" s="1" t="s">
         <v>130</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>132</v>
       </c>
       <c r="F7" s="1" t="s">
         <v>5</v>
@@ -1212,7 +1212,7 @@
         <v>10</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="E8" s="1" t="s">
         <v>7</v>
@@ -1238,13 +1238,13 @@
         <v>12</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
@@ -1255,19 +1255,19 @@
         <v>5</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>13</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
@@ -1350,7 +1350,7 @@
         <v>23</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="E14" s="1" t="s">
         <v>24</v>
@@ -1379,10 +1379,10 @@
         <v>28</v>
       </c>
       <c r="F15" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.3">
@@ -1494,10 +1494,10 @@
         <v>24</v>
       </c>
       <c r="F20" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.3">
@@ -1520,7 +1520,7 @@
         <v>39</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.3">
@@ -1606,13 +1606,13 @@
         <v>51</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="G25" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.3">
@@ -1632,10 +1632,10 @@
         <v>55</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.3">
@@ -1689,13 +1689,13 @@
         <v>2</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>60</v>
+        <v>194</v>
       </c>
       <c r="C29" s="1" t="s">
         <v>23</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E29" s="1" t="s">
         <v>24</v>
@@ -1712,13 +1712,13 @@
         <v>2</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C30" s="1" t="s">
         <v>15</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E30" s="1" t="s">
         <v>17</v>
@@ -1735,22 +1735,22 @@
         <v>1</v>
       </c>
       <c r="B31" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="C31" t="s">
+        <v>171</v>
+      </c>
+      <c r="D31" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="C31" t="s">
-        <v>175</v>
-      </c>
-      <c r="D31" s="1" t="s">
+      <c r="E31" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="E31" s="1" t="s">
-        <v>66</v>
-      </c>
       <c r="F31" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="G31" s="1" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.3">
@@ -1758,22 +1758,22 @@
         <v>1</v>
       </c>
       <c r="B32" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="C32" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="C32" s="1" t="s">
+      <c r="D32" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="D32" s="1" t="s">
+      <c r="E32" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="E32" s="1" t="s">
-        <v>70</v>
-      </c>
       <c r="F32" s="1" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="G32" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.3">
@@ -1781,13 +1781,13 @@
         <v>4</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C33" s="1" t="s">
         <v>23</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E33" s="1" t="s">
         <v>24</v>
@@ -1804,13 +1804,13 @@
         <v>1</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>73</v>
+        <v>193</v>
       </c>
       <c r="C34" s="1" t="s">
         <v>15</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="E34" s="1" t="s">
         <v>17</v>
@@ -1827,13 +1827,13 @@
         <v>4</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C35" s="1" t="s">
         <v>15</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="E35" s="1" t="s">
         <v>17</v>
@@ -1850,13 +1850,13 @@
         <v>7</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C36" s="1" t="s">
         <v>15</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="E36" s="1" t="s">
         <v>17</v>
@@ -1873,13 +1873,13 @@
         <v>1</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C37" s="1" t="s">
         <v>15</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="E37" s="1" t="s">
         <v>17</v>
@@ -1896,13 +1896,13 @@
         <v>2</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C38" s="1" t="s">
         <v>15</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="E38" s="1" t="s">
         <v>17</v>
@@ -1919,22 +1919,22 @@
         <v>1</v>
       </c>
       <c r="B39" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="C39" t="s">
+        <v>172</v>
+      </c>
+      <c r="D39" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="E39" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="C39" t="s">
-        <v>176</v>
-      </c>
-      <c r="D39" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="E39" s="1" t="s">
-        <v>85</v>
-      </c>
       <c r="F39" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="G39" s="1" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.3">
@@ -1942,16 +1942,16 @@
         <v>4</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="E40" s="1" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="F40" s="1" t="s">
         <v>5</v>
@@ -1965,22 +1965,22 @@
         <v>1</v>
       </c>
       <c r="B41" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="D41" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="C41" s="1" t="s">
+      <c r="E41" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="D41" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="E41" s="1" t="s">
-        <v>91</v>
-      </c>
       <c r="F41" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="G41" s="1" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.3">
@@ -1988,16 +1988,16 @@
         <v>1</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="F42" s="1"/>
       <c r="G42" s="1" t="s">
@@ -2009,22 +2009,22 @@
         <v>1</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="E43" s="1" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="F43" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="G43" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.3">
@@ -2032,16 +2032,16 @@
         <v>2</v>
       </c>
       <c r="B44" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="C44" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="D44" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="C44" s="1" t="s">
+      <c r="E44" s="1" t="s">
         <v>98</v>
-      </c>
-      <c r="D44" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="E44" s="1" t="s">
-        <v>100</v>
       </c>
       <c r="F44" s="1" t="s">
         <v>5</v>
@@ -2055,19 +2055,19 @@
         <v>1</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="E45" s="1" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="F45" s="1" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="G45" s="1" t="s">
         <v>5</v>
@@ -2078,22 +2078,22 @@
         <v>1</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="E46" s="1" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="F46" s="1" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="G46" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.3">
@@ -2101,22 +2101,22 @@
         <v>1</v>
       </c>
       <c r="B47" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="C47" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="D47" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="C47" s="1" t="s">
+      <c r="E47" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="D47" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="E47" s="1" t="s">
-        <v>109</v>
-      </c>
       <c r="F47" s="1" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="G47" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.3">
@@ -2124,22 +2124,22 @@
         <v>1</v>
       </c>
       <c r="B48" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="C48" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="D48" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="C48" s="1" t="s">
+      <c r="E48" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="D48" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="E48" s="1" t="s">
-        <v>113</v>
-      </c>
       <c r="F48" s="1" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="G48" s="1" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.3">
@@ -2147,16 +2147,16 @@
         <v>2</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="C49" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="D49" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="E49" s="1" t="s">
         <v>98</v>
-      </c>
-      <c r="D49" s="1" t="s">
-        <v>115</v>
-      </c>
-      <c r="E49" s="1" t="s">
-        <v>100</v>
       </c>
       <c r="F49" s="1" t="s">
         <v>5</v>
@@ -2170,19 +2170,19 @@
         <v>1</v>
       </c>
       <c r="B50" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="C50" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="D50" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="C50" s="1" t="s">
-        <v>117</v>
-      </c>
-      <c r="D50" s="1" t="s">
-        <v>118</v>
-      </c>
       <c r="E50" s="1" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="F50" s="1" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="G50" s="1" t="s">
         <v>5</v>
@@ -2193,22 +2193,22 @@
         <v>1</v>
       </c>
       <c r="B51" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="C51" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="D51" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="C51" s="1" t="s">
+      <c r="E51" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="D51" s="1" t="s">
-        <v>121</v>
-      </c>
-      <c r="E51" s="1" t="s">
-        <v>122</v>
-      </c>
       <c r="F51" s="1" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="G51" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.3">
@@ -2216,13 +2216,13 @@
         <v>1</v>
       </c>
       <c r="B52" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="C52" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="D52" s="1" t="s">
         <v>123</v>
-      </c>
-      <c r="C52" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="D52" s="1" t="s">
-        <v>125</v>
       </c>
       <c r="E52" s="1" t="s">
         <v>5</v>
@@ -2239,22 +2239,22 @@
         <v>4</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>144</v>
+        <v>195</v>
       </c>
       <c r="E53" s="1" t="s">
-        <v>135</v>
+        <v>196</v>
       </c>
       <c r="F53" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="G53" s="1" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.3">
@@ -2262,16 +2262,16 @@
         <v>1</v>
       </c>
       <c r="B54" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="C54" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="D54" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="C54" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="D54" s="1" t="s">
-        <v>128</v>
-      </c>
       <c r="E54" s="1" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="F54" s="1" t="s">
         <v>5</v>
@@ -2285,22 +2285,22 @@
         <v>1</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="D55" s="1" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="E55" s="1" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="F55" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="G55" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
     </row>
   </sheetData>

</xml_diff>